<commit_message>
Update lexicon: remove syntax category
</commit_message>
<xml_diff>
--- a/vocabulary/lexicon.xlsx
+++ b/vocabulary/lexicon.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="232">
   <si>
     <t xml:space="preserve">slug</t>
   </si>
@@ -51,12 +51,6 @@
   </si>
   <si>
     <t xml:space="preserve">Morphosyntax</t>
-  </si>
-  <si>
-    <t xml:space="preserve">syntax</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Syntax</t>
   </si>
   <si>
     <t xml:space="preserve">syntactic-construction</t>
@@ -1068,14 +1062,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1103,16 +1090,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.76"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1121,10 +1108,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1132,10 +1119,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E2" s="2"/>
     </row>
@@ -1144,13 +1131,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -1159,13 +1146,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -1174,10 +1161,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -1186,10 +1173,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -1198,10 +1185,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -1210,13 +1197,13 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -1225,10 +1212,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -1237,13 +1224,13 @@
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -1252,10 +1239,10 @@
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -1264,13 +1251,13 @@
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E12" s="2"/>
     </row>
@@ -1279,13 +1266,13 @@
         <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E13" s="2"/>
     </row>
@@ -1294,10 +1281,10 @@
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -1306,10 +1293,10 @@
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E15" s="2"/>
     </row>
@@ -1318,13 +1305,13 @@
         <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E16" s="2"/>
     </row>
@@ -1333,10 +1320,10 @@
         <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E17" s="2"/>
     </row>
@@ -1345,10 +1332,10 @@
         <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E18" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -1360,13 +1347,13 @@
         <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E19" s="2"/>
     </row>
@@ -1375,13 +1362,13 @@
         <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E20" s="2"/>
     </row>
@@ -1390,13 +1377,13 @@
         <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E21" s="2"/>
     </row>
@@ -1405,13 +1392,13 @@
         <v>2</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E22" s="2"/>
     </row>
@@ -1420,13 +1407,13 @@
         <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E23" s="2"/>
     </row>
@@ -1435,13 +1422,13 @@
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E24" s="2"/>
     </row>
@@ -1450,10 +1437,10 @@
         <v>2</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E25" s="2"/>
     </row>
@@ -1462,10 +1449,10 @@
         <v>2</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E26" s="2"/>
     </row>
@@ -1474,13 +1461,13 @@
         <v>2</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E27" s="2"/>
     </row>
@@ -1489,10 +1476,10 @@
         <v>2</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E28" s="2"/>
     </row>
@@ -1501,10 +1488,10 @@
         <v>2</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E29" s="2"/>
     </row>
@@ -1513,13 +1500,13 @@
         <v>2</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E30" s="2"/>
     </row>
@@ -1528,13 +1515,13 @@
         <v>2</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E31" s="2"/>
     </row>
@@ -1543,10 +1530,10 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1554,10 +1541,10 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1565,13 +1552,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1579,13 +1566,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1593,13 +1580,13 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1607,13 +1594,13 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1621,10 +1608,10 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1632,10 +1619,10 @@
         <v>4</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1643,10 +1630,10 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1654,10 +1641,10 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1665,10 +1652,10 @@
         <v>4</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1676,10 +1663,10 @@
         <v>4</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1687,10 +1674,10 @@
         <v>4</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1698,10 +1685,10 @@
         <v>4</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1709,10 +1696,10 @@
         <v>4</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1720,10 +1707,10 @@
         <v>4</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1731,13 +1718,13 @@
         <v>4</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1745,13 +1732,13 @@
         <v>4</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1759,10 +1746,10 @@
         <v>4</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1770,10 +1757,10 @@
         <v>4</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1781,10 +1768,10 @@
         <v>4</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1792,10 +1779,10 @@
         <v>4</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1803,10 +1790,10 @@
         <v>6</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1814,10 +1801,10 @@
         <v>6</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1825,10 +1812,10 @@
         <v>6</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1836,10 +1823,10 @@
         <v>6</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1847,10 +1834,10 @@
         <v>6</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1858,10 +1845,10 @@
         <v>6</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1869,10 +1856,10 @@
         <v>6</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1880,10 +1867,10 @@
         <v>8</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1891,10 +1878,10 @@
         <v>8</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1902,10 +1889,10 @@
         <v>8</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1913,10 +1900,10 @@
         <v>8</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1924,10 +1911,10 @@
         <v>8</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1935,10 +1922,10 @@
         <v>8</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1946,10 +1933,10 @@
         <v>8</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1957,10 +1944,10 @@
         <v>8</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1968,10 +1955,10 @@
         <v>8</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1979,13 +1966,13 @@
         <v>8</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1993,13 +1980,13 @@
         <v>8</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2007,13 +1994,13 @@
         <v>8</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2021,13 +2008,13 @@
         <v>8</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2035,13 +2022,13 @@
         <v>8</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2049,13 +2036,13 @@
         <v>8</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2063,13 +2050,13 @@
         <v>8</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2077,13 +2064,13 @@
         <v>8</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2091,13 +2078,13 @@
         <v>8</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2105,13 +2092,13 @@
         <v>8</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2119,13 +2106,13 @@
         <v>8</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2133,13 +2120,13 @@
         <v>8</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2147,13 +2134,13 @@
         <v>8</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2161,13 +2148,13 @@
         <v>8</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2175,13 +2162,13 @@
         <v>8</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2189,13 +2176,13 @@
         <v>8</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2203,13 +2190,13 @@
         <v>8</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2217,13 +2204,13 @@
         <v>8</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2231,13 +2218,13 @@
         <v>8</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2245,13 +2232,13 @@
         <v>8</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2259,13 +2246,13 @@
         <v>8</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2273,13 +2260,13 @@
         <v>8</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2287,13 +2274,13 @@
         <v>8</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2301,13 +2288,13 @@
         <v>8</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2315,13 +2302,13 @@
         <v>8</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2329,13 +2316,13 @@
         <v>8</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2343,13 +2330,13 @@
         <v>8</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2357,13 +2344,13 @@
         <v>8</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2371,13 +2358,13 @@
         <v>8</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2385,13 +2372,13 @@
         <v>8</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2399,13 +2386,13 @@
         <v>8</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2413,13 +2400,13 @@
         <v>8</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2427,13 +2414,13 @@
         <v>8</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2441,105 +2428,105 @@
         <v>8</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add ULL and CCR terms and links
</commit_message>
<xml_diff>
--- a/vocabulary/lexicon.xlsx
+++ b/vocabulary/lexicon.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="categories" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="376">
   <si>
     <t xml:space="preserve">slug</t>
   </si>
@@ -74,42 +74,84 @@
     <t xml:space="preserve">selectable</t>
   </si>
   <si>
+    <t xml:space="preserve">ull</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ull-url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ccr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ccr-url</t>
+  </si>
+  <si>
     <t xml:space="preserve">noun</t>
   </si>
   <si>
     <t xml:space="preserve">Noun</t>
   </si>
   <si>
+    <t xml:space="preserve">https://lexicon.hum.uu.nl/zoek.pl?lemma=Noun+(N)&amp;lemmacode=509</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-3347_7face0f5-7a72-7ec2-c988-7adba256cea9</t>
+  </si>
+  <si>
     <t xml:space="preserve">proper-noun</t>
   </si>
   <si>
     <t xml:space="preserve">Proper noun</t>
   </si>
   <si>
+    <t xml:space="preserve">proper noun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1371_fbebd9ec-a7f4-9a36-d6e9-88ee16b944ae </t>
+  </si>
+  <si>
     <t xml:space="preserve">common-noun</t>
   </si>
   <si>
     <t xml:space="preserve">Common noun</t>
   </si>
   <si>
+    <t xml:space="preserve">common noun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-385_d5af2f91-c926-3747-cc35-1d21aefd2717 </t>
+  </si>
+  <si>
     <t xml:space="preserve">verb</t>
   </si>
   <si>
     <t xml:space="preserve">Verb</t>
   </si>
   <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1424_dc8402e6-a042-2d8a-4740-0d6cfe5ede02</t>
+  </si>
+  <si>
     <t xml:space="preserve">adjective</t>
   </si>
   <si>
     <t xml:space="preserve">Adjective</t>
   </si>
   <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-4948_ed655357-4652-f480-1a1e-a2999b785608</t>
+  </si>
+  <si>
     <t xml:space="preserve">adverb</t>
   </si>
   <si>
     <t xml:space="preserve">Adverb</t>
   </si>
   <si>
+    <t xml:space="preserve">https://lexicon.hum.uu.nl/zoek.pl?lemma=Adverb&amp;lemmacode=992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-4955_80fe4ee9-ea7e-527a-a860-b7956c95e1f8</t>
+  </si>
+  <si>
     <t xml:space="preserve">preposition</t>
   </si>
   <si>
@@ -119,57 +161,108 @@
     <t xml:space="preserve">adposition</t>
   </si>
   <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-3419_28e9d227-d7f2-1ef7-a8a6-064c04dbdb4e</t>
+  </si>
+  <si>
     <t xml:space="preserve">Adposition</t>
   </si>
   <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1231_254a8099-18bf-fd87-781e-9dd5e5129c37</t>
+  </si>
+  <si>
     <t xml:space="preserve">postposition</t>
   </si>
   <si>
     <t xml:space="preserve">Postposition</t>
   </si>
   <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1360_dc07e05a-b7bf-7e3e-360b-3d1e2a5c1c7f</t>
+  </si>
+  <si>
     <t xml:space="preserve">numeral</t>
   </si>
   <si>
     <t xml:space="preserve">Numeral</t>
   </si>
   <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1334_3ef89474-3670-161f-6212-beb82406bb75</t>
+  </si>
+  <si>
     <t xml:space="preserve">cardinal</t>
   </si>
   <si>
     <t xml:space="preserve">Cardinal</t>
   </si>
   <si>
+    <t xml:space="preserve">CardinalNumeral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-3103_2703f461-5695-5fe4-46bd-bcb6d40d19c0</t>
+  </si>
+  <si>
     <t xml:space="preserve">ordinal</t>
   </si>
   <si>
     <t xml:space="preserve">Ordinal</t>
   </si>
   <si>
+    <t xml:space="preserve">OrdinalNumeral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-3361_1af3740e-1092-c02a-2038-9428ddcddd7b</t>
+  </si>
+  <si>
     <t xml:space="preserve">particle</t>
   </si>
   <si>
     <t xml:space="preserve">Particle</t>
   </si>
   <si>
+    <t xml:space="preserve">https://lexicon.hum.uu.nl/zoek.pl?lemma=Particle&amp;lemmacode=382</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-3372_8d6a8199-b259-537e-fbca-5de0aa46d7f9</t>
+  </si>
+  <si>
     <t xml:space="preserve">pronoun</t>
   </si>
   <si>
     <t xml:space="preserve">Pronoun</t>
   </si>
   <si>
+    <t xml:space="preserve">pronominal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://lexicon.hum.uu.nl/zoek.pl?lemma=Pronominal&amp;lemmacode=447</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-4951_3b095c38-b7d9-6903-267b-5ab6a7812459</t>
+  </si>
+  <si>
     <t xml:space="preserve">personal-pronoun</t>
   </si>
   <si>
     <t xml:space="preserve">Personal pronoun</t>
   </si>
   <si>
+    <t xml:space="preserve">personal pronoun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1463_f07c7667-e90f-c10a-7239-1ecb8d804956 </t>
+  </si>
+  <si>
     <t xml:space="preserve">determiner</t>
   </si>
   <si>
     <t xml:space="preserve">Determiner</t>
   </si>
   <si>
+    <t xml:space="preserve">https://lexicon.hum.uu.nl/zoek.pl?lemma=Determiner&amp;lemmacode=1079</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-3159_a027395b-0971-f4d3-52d5-f42dd670a655</t>
+  </si>
+  <si>
     <t xml:space="preserve">pronoun-determiner</t>
   </si>
   <si>
@@ -182,36 +275,87 @@
     <t xml:space="preserve">Relative pronoun</t>
   </si>
   <si>
+    <t xml:space="preserve">relative pronoun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://lexicon.hum.uu.nl/zoek.pl?lemma=Relative+pronoun&amp;lemmacode=332</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1380_e55f8cdf-1792-eb7a-6792-4e6c9b3c176a</t>
+  </si>
+  <si>
     <t xml:space="preserve">reflexive-pronoun</t>
   </si>
   <si>
     <t xml:space="preserve">Reflexive pronoun</t>
   </si>
   <si>
+    <t xml:space="preserve">reflexive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://lexicon.hum.uu.nl/zoek.pl?lemma=Reflexive&amp;lemmacode=329</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reflexive personal pronoun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-3014_e837f69a-cc20-0fe6-a94a-153e8f59b694</t>
+  </si>
+  <si>
     <t xml:space="preserve">reciprocal-pronoun</t>
   </si>
   <si>
     <t xml:space="preserve">Reciprocal pronoun</t>
   </si>
   <si>
+    <t xml:space="preserve">reciprocal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://lexicon.hum.uu.nl/zoek.pl?lemma=Reciprocal&amp;lemmacode=316</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reciprocal pronoun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-4986_c70204a7-79a7-b916-3cfb-1572cde565f8</t>
+  </si>
+  <si>
     <t xml:space="preserve">demonstrative-pronoun</t>
   </si>
   <si>
     <t xml:space="preserve">Demonstrative pronoun</t>
   </si>
   <si>
+    <t xml:space="preserve">demonstrative pronoun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1270_bfb2e942-c2a8-1035-cde9-b8ada8c9aa70</t>
+  </si>
+  <si>
     <t xml:space="preserve">interrogative-pronoun</t>
   </si>
   <si>
     <t xml:space="preserve">Interrogative pronoun</t>
   </si>
   <si>
+    <t xml:space="preserve">interrogative pronoun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1321_35cb0c2b-aa78-024b-9e6b-ae2a94cb191c</t>
+  </si>
+  <si>
     <t xml:space="preserve">possessive-pronoun</t>
   </si>
   <si>
     <t xml:space="preserve">Possessive pronoun</t>
   </si>
   <si>
+    <t xml:space="preserve">possessive pronoun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1359_41a180fd-f9a4-25e3-25c1-69c1225c31c8 </t>
+  </si>
+  <si>
     <t xml:space="preserve">article</t>
   </si>
   <si>
@@ -224,6 +368,9 @@
     <t xml:space="preserve">Symbol</t>
   </si>
   <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-5037_12ebd479-c44e-1e62-938e-38890ca17ef0</t>
+  </si>
+  <si>
     <t xml:space="preserve">punctuation-symbol</t>
   </si>
   <si>
@@ -236,42 +383,78 @@
     <t xml:space="preserve">Interjection</t>
   </si>
   <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-3266_382e27ef-820b-8861-5aa3-b60dbe69936e</t>
+  </si>
+  <si>
     <t xml:space="preserve">conjunction</t>
   </si>
   <si>
     <t xml:space="preserve">Conjunction</t>
   </si>
   <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-3132_60542513-24d3-973f-9dd6-678d372e5aa7</t>
+  </si>
+  <si>
     <t xml:space="preserve">coordinate-conjunction</t>
   </si>
   <si>
     <t xml:space="preserve">Coordinate conjunction</t>
   </si>
   <si>
+    <t xml:space="preserve">coordinating conjunction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1262_64a7cd7c-4e1e-ac0a-0ee0-ac1541f27aea</t>
+  </si>
+  <si>
     <t xml:space="preserve">subordinate-conjunction</t>
   </si>
   <si>
     <t xml:space="preserve">Subordinate conjunction</t>
   </si>
   <si>
+    <t xml:space="preserve">complementizer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://lexicon.hum.uu.nl/zoek.pl?lemma=Complementizer&amp;lemmacode=892</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subordinating conjunction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1393_9905e94f-5624-ed01-139f-fc3ffac7a923</t>
+  </si>
+  <si>
     <t xml:space="preserve">subject</t>
   </si>
   <si>
     <t xml:space="preserve">Subject</t>
   </si>
   <si>
+    <t xml:space="preserve">https://lexicon.hum.uu.nl/zoek.pl?lemma=Subject&amp;lemmacode=285</t>
+  </si>
+  <si>
     <t xml:space="preserve">object</t>
   </si>
   <si>
     <t xml:space="preserve">Object</t>
   </si>
   <si>
+    <t xml:space="preserve">https://lexicon.hum.uu.nl/zoek.pl?lemma=Object&amp;lemmacode=462</t>
+  </si>
+  <si>
     <t xml:space="preserve">direct-object</t>
   </si>
   <si>
     <t xml:space="preserve">Direct object</t>
   </si>
   <si>
+    <t xml:space="preserve">direct object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1274_2d458147-53dc-9010-d77b-3a3d6a0aeb49</t>
+  </si>
+  <si>
     <t xml:space="preserve">primary-object</t>
   </si>
   <si>
@@ -290,6 +473,12 @@
     <t xml:space="preserve">Indirect object</t>
   </si>
   <si>
+    <t xml:space="preserve">indirect object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1310_ab441fcb-3588-e2c8-14ed-45e22106df1f</t>
+  </si>
+  <si>
     <t xml:space="preserve">predicate</t>
   </si>
   <si>
@@ -302,6 +491,12 @@
     <t xml:space="preserve">Prepositional complement</t>
   </si>
   <si>
+    <t xml:space="preserve">prepositional Complement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-4638_49e9d219-69c9-5391-2c85-67ae442761d6</t>
+  </si>
+  <si>
     <t xml:space="preserve">clausal-complement</t>
   </si>
   <si>
@@ -314,12 +509,21 @@
     <t xml:space="preserve">Modifier</t>
   </si>
   <si>
+    <t xml:space="preserve">https://lexicon.hum.uu.nl/zoek.pl?lemma=Modifier&amp;lemmacode=553</t>
+  </si>
+  <si>
     <t xml:space="preserve">secondary-predicate</t>
   </si>
   <si>
     <t xml:space="preserve">Secondary predicate</t>
   </si>
   <si>
+    <t xml:space="preserve">secondary predicate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-5454_aea7d73d-4cd2-4e36-0229-a009162e05ce</t>
+  </si>
+  <si>
     <t xml:space="preserve">locative-directional-complement</t>
   </si>
   <si>
@@ -338,6 +542,12 @@
     <t xml:space="preserve">Head</t>
   </si>
   <si>
+    <t xml:space="preserve">nucleus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-357_c6bf01ef-e8cf-e88c-00e3-ac24d21fefb7</t>
+  </si>
+  <si>
     <t xml:space="preserve">determiner-relation</t>
   </si>
   <si>
@@ -380,9 +590,6 @@
     <t xml:space="preserve">Coordinator</t>
   </si>
   <si>
-    <t xml:space="preserve">complementizer</t>
-  </si>
-  <si>
     <t xml:space="preserve">Complementizer</t>
   </si>
   <si>
@@ -392,24 +599,48 @@
     <t xml:space="preserve">Noun phrase</t>
   </si>
   <si>
+    <t xml:space="preserve">noun phrase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-2256_f31b9b2c-03a2-2251-10d4-7d98ddc042b0</t>
+  </si>
+  <si>
     <t xml:space="preserve">adjective-phrase</t>
   </si>
   <si>
     <t xml:space="preserve">Adjective phrase</t>
   </si>
   <si>
+    <t xml:space="preserve">adjective phrase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-2258_121366f1-07d0-2c34-373d-342e4d637446 </t>
+  </si>
+  <si>
     <t xml:space="preserve">prepositional-phrase</t>
   </si>
   <si>
     <t xml:space="preserve">Prepositional phrase</t>
   </si>
   <si>
+    <t xml:space="preserve">prepositional phrase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-5768_1e635399-e84b-b206-6ece-4e573a30ca18 </t>
+  </si>
+  <si>
     <t xml:space="preserve">verb-phrase</t>
   </si>
   <si>
     <t xml:space="preserve">Verb phrase</t>
   </si>
   <si>
+    <t xml:space="preserve">verb phrase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-2255_88b411af-49bf-1cdb-7aad-224eb27ef06f</t>
+  </si>
+  <si>
     <t xml:space="preserve">adpositional-phrase</t>
   </si>
   <si>
@@ -422,6 +653,12 @@
     <t xml:space="preserve">Adverb phrase</t>
   </si>
   <si>
+    <t xml:space="preserve">adverb phrase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-2259_a44e604a-d29f-3d22-68d9-3c578de7d057</t>
+  </si>
+  <si>
     <t xml:space="preserve">determiner-phrase</t>
   </si>
   <si>
@@ -434,132 +671,243 @@
     <t xml:space="preserve">Mood</t>
   </si>
   <si>
+    <t xml:space="preserve">https://lexicon.hum.uu.nl/zoek.pl?lemma=Mood&amp;lemmacode=559 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">verb form mood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1427_a6c3919f-4cc1-9d38-f431-3f44e45d0104 </t>
+  </si>
+  <si>
     <t xml:space="preserve">tense</t>
   </si>
   <si>
     <t xml:space="preserve">Tense</t>
   </si>
   <si>
+    <t xml:space="preserve">https://lexicon.hum.uu.nl/zoek.pl?lemma=Tense&amp;lemmacode=144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1286_6bf93a88-ee71-1487-5de5-d7ca9c1f4397 </t>
+  </si>
+  <si>
     <t xml:space="preserve">aspect</t>
   </si>
   <si>
     <t xml:space="preserve">Aspect</t>
   </si>
   <si>
+    <t xml:space="preserve">https://lexicon.hum.uu.nl/zoek.pl?lemma=Aspect&amp;lemmacode=1041</t>
+  </si>
+  <si>
     <t xml:space="preserve">person</t>
   </si>
   <si>
     <t xml:space="preserve">Person</t>
   </si>
   <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-2775_0d862930-ad75-39db-21c5-7aeeef08b3c3 </t>
+  </si>
+  <si>
     <t xml:space="preserve">number</t>
   </si>
   <si>
     <t xml:space="preserve">Number</t>
   </si>
   <si>
+    <t xml:space="preserve">https://lexicon.hum.uu.nl/zoek.pl?lemma=Number&amp;lemmacode=518</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-2709_cb240da0-9009-d7cf-4a7d-76c82bd9d571 </t>
+  </si>
+  <si>
     <t xml:space="preserve">gender</t>
   </si>
   <si>
     <t xml:space="preserve">Gender</t>
   </si>
   <si>
+    <t xml:space="preserve">https://lexicon.hum.uu.nl/zoek.pl?lemma=Gender&amp;lemmacode=716</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-4926_08350667-c77d-15cb-2273-066dfba297c4 </t>
+  </si>
+  <si>
     <t xml:space="preserve">definiteness</t>
   </si>
   <si>
     <t xml:space="preserve">Definiteness</t>
   </si>
   <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1926_54336616-beda-d9e9-c1e8-28f8233e8f7f </t>
+  </si>
+  <si>
     <t xml:space="preserve">case</t>
   </si>
   <si>
     <t xml:space="preserve">Case</t>
   </si>
   <si>
+    <t xml:space="preserve">https://lexicon.hum.uu.nl/zoek.pl?lemma=Case&amp;lemmacode=854</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1840_9f4e319c-f233-6c90-9117-7270e215f039 </t>
+  </si>
+  <si>
     <t xml:space="preserve">degree</t>
   </si>
   <si>
     <t xml:space="preserve">Degree</t>
   </si>
   <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-4920_305a6674-d773-1ab4-2deb-66871c089fff </t>
+  </si>
+  <si>
     <t xml:space="preserve">indicative</t>
   </si>
   <si>
     <t xml:space="preserve">Indicative</t>
   </si>
   <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1885_9db4ec86-e0c3-91d9-4365-4eec106b5126</t>
+  </si>
+  <si>
     <t xml:space="preserve">subjunctive</t>
   </si>
   <si>
     <t xml:space="preserve">Subjunctive</t>
   </si>
   <si>
+    <t xml:space="preserve">https://lexicon.hum.uu.nl/zoek.pl?lemma=Subjunctive&amp;lemmacode=291</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1843_a492ced1-dbba-d8d8-1d8a-71387ede8a48</t>
+  </si>
+  <si>
     <t xml:space="preserve">conjunctive</t>
   </si>
   <si>
     <t xml:space="preserve">Conjunctive</t>
   </si>
   <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-4967_f065b067-9908-dfd2-9397-27261b8e17d0 </t>
+  </si>
+  <si>
     <t xml:space="preserve">imperative</t>
   </si>
   <si>
     <t xml:space="preserve">Imperative</t>
   </si>
   <si>
+    <t xml:space="preserve">https://lexicon.hum.uu.nl/zoek.pl?lemma=Imperative&amp;lemmacode=652</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1844_21036bac-13d1-18fc-ca4f-2590f5c84013 </t>
+  </si>
+  <si>
     <t xml:space="preserve">present-tense</t>
   </si>
   <si>
     <t xml:space="preserve">Present tense</t>
   </si>
   <si>
+    <t xml:space="preserve">present</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-4965_703be00b-9336-3673-0f2d-d274352dd15e </t>
+  </si>
+  <si>
     <t xml:space="preserve">past-tense</t>
   </si>
   <si>
     <t xml:space="preserve">Past tense</t>
   </si>
   <si>
+    <t xml:space="preserve">past</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-4966_7a720367-df40-f728-e11d-7504a03ec27b </t>
+  </si>
+  <si>
     <t xml:space="preserve">future-tense</t>
   </si>
   <si>
     <t xml:space="preserve">Future tense</t>
   </si>
   <si>
+    <t xml:space="preserve">future</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1291_c2896356-8d7e-e425-d2ac-5741e93db4e2 </t>
+  </si>
+  <si>
     <t xml:space="preserve">imperfective</t>
   </si>
   <si>
     <t xml:space="preserve">Imperfective</t>
   </si>
   <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1305_7066f625-844d-7091-167c-1770bb560b7e </t>
+  </si>
+  <si>
     <t xml:space="preserve">perfective</t>
   </si>
   <si>
     <t xml:space="preserve">Perfective</t>
   </si>
   <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1352_2664f3ef-8d98-764f-9ec5-d582ed04d312 </t>
+  </si>
+  <si>
     <t xml:space="preserve">first-person</t>
   </si>
   <si>
     <t xml:space="preserve">First person</t>
   </si>
   <si>
+    <t xml:space="preserve">first person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1288_61cc5804-ed04-b31a-d550-7fe84a188345 </t>
+  </si>
+  <si>
     <t xml:space="preserve">second-person</t>
   </si>
   <si>
     <t xml:space="preserve">Second person</t>
   </si>
   <si>
+    <t xml:space="preserve">second person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1384_a6aa56c1-3f5d-901f-cbbb-ecc8fdce9d69 </t>
+  </si>
+  <si>
     <t xml:space="preserve">third-person</t>
   </si>
   <si>
     <t xml:space="preserve">Third person</t>
   </si>
   <si>
+    <t xml:space="preserve">third person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1402_fd8749a9-cd4a-530e-760e-17944acfd054 </t>
+  </si>
+  <si>
     <t xml:space="preserve">singular</t>
   </si>
   <si>
     <t xml:space="preserve">Singular</t>
   </si>
   <si>
+    <t xml:space="preserve">singular number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-2707_9c804dcc-7939-8f37-d4d4-10423ee65e20 </t>
+  </si>
+  <si>
     <t xml:space="preserve">dual</t>
   </si>
   <si>
@@ -578,72 +926,135 @@
     <t xml:space="preserve">Plural</t>
   </si>
   <si>
+    <t xml:space="preserve">plural number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-2708_74a6e5d5-6df6-7756-c882-ce09731285eb </t>
+  </si>
+  <si>
     <t xml:space="preserve">masculine</t>
   </si>
   <si>
     <t xml:space="preserve">Masculine</t>
   </si>
   <si>
+    <t xml:space="preserve">MasculineGender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-3312_4e7c6a3d-3b48-8ade-de52-cfaa9122269a </t>
+  </si>
+  <si>
     <t xml:space="preserve">feminine</t>
   </si>
   <si>
     <t xml:space="preserve">Feminine</t>
   </si>
   <si>
+    <t xml:space="preserve">FeminineGender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-3197_9e0c49be-b888-bc56-b6d1-05f4dd1d5a66 </t>
+  </si>
+  <si>
     <t xml:space="preserve">neuter</t>
   </si>
   <si>
     <t xml:space="preserve">Neuter</t>
   </si>
   <si>
+    <t xml:space="preserve">NeuterGender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-3336_086f7d13-1e1c-8618-5051-b9c7ab4cf860 </t>
+  </si>
+  <si>
     <t xml:space="preserve">uter</t>
   </si>
   <si>
     <t xml:space="preserve">Uter</t>
   </si>
   <si>
+    <t xml:space="preserve">common gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1558_015e4ddd-aff5-d9ec-ec64-e6be2c029456 </t>
+  </si>
+  <si>
     <t xml:space="preserve">definite</t>
   </si>
   <si>
     <t xml:space="preserve">Definite</t>
   </si>
   <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-2004_7dc427d7-61a6-853e-12ea-c7f766afc5b6 </t>
+  </si>
+  <si>
     <t xml:space="preserve">indefinite</t>
   </si>
   <si>
     <t xml:space="preserve">Indefinite</t>
   </si>
   <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-2005_05c694a1-bf78-c5bc-4913-a87f7b30f251 </t>
+  </si>
+  <si>
     <t xml:space="preserve">nominative</t>
   </si>
   <si>
     <t xml:space="preserve">Nominative</t>
   </si>
   <si>
+    <t xml:space="preserve">nominative case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1331_89e7297d-85b0-5391-ea92-92347358719d </t>
+  </si>
+  <si>
     <t xml:space="preserve">accusative</t>
   </si>
   <si>
     <t xml:space="preserve">Accusative</t>
   </si>
   <si>
+    <t xml:space="preserve">accusative case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-2724_53acfdbe-6741-7430-6e7f-677b47993c17 </t>
+  </si>
+  <si>
     <t xml:space="preserve">genitive</t>
   </si>
   <si>
     <t xml:space="preserve">Genitive</t>
   </si>
   <si>
+    <t xml:space="preserve">genitive case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1293_5ce1a413-afaf-1ae5-f818-a416f219fc41 </t>
+  </si>
+  <si>
     <t xml:space="preserve">dative</t>
   </si>
   <si>
     <t xml:space="preserve">Dative</t>
   </si>
   <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-4938_8d013ba9-c95a-ec59-6cc9-ed61e2cff5f1 </t>
+  </si>
+  <si>
     <t xml:space="preserve">locative</t>
   </si>
   <si>
     <t xml:space="preserve">Locative</t>
   </si>
   <si>
+    <t xml:space="preserve">locative case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-2726_da687347-23ae-062f-92c5-af3acf7d6b82 </t>
+  </si>
+  <si>
     <t xml:space="preserve">prepositionalis</t>
   </si>
   <si>
@@ -662,22 +1073,43 @@
     <t xml:space="preserve">Positive</t>
   </si>
   <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1420_745016c4-84c2-766a-a861-b4cdb6dcba73 </t>
+  </si>
+  <si>
     <t xml:space="preserve">comparative</t>
   </si>
   <si>
     <t xml:space="preserve">Comparative</t>
   </si>
   <si>
+    <t xml:space="preserve">https://lexicon.hum.uu.nl/zoek.pl?lemma=comparative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-4924_1867b087-ed2e-1641-4948-6753bc5c439a </t>
+  </si>
+  <si>
     <t xml:space="preserve">superlative</t>
   </si>
   <si>
     <t xml:space="preserve">Superlative</t>
   </si>
   <si>
+    <t xml:space="preserve">https://lexicon.hum.uu.nl/zoek.pl?lemma=Superlative&amp;lemmacode=299</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-4925_fe8c3b92-8af1-70e2-2534-923b977ac4e8 </t>
+  </si>
+  <si>
     <t xml:space="preserve">diminutive</t>
   </si>
   <si>
     <t xml:space="preserve">Diminutive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://lexicon.hum.uu.nl/zoek.pl?lemma=Diminutive&amp;lemmacode=1081</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-3046_73e3fbc4-0fc7-513e-d225-517203331e74 </t>
   </si>
   <si>
     <t xml:space="preserve">augmentative</t>
@@ -727,7 +1159,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;WAAR&quot;;&quot;WAAR&quot;;&quot;ONWAAR&quot;"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -748,6 +1180,20 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -792,7 +1238,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -801,7 +1247,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -996,7 +1458,7 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1080,12 +1542,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E110"/>
+  <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E107" activeCellId="0" sqref="E107"/>
+      <selection pane="bottomLeft" activeCell="G113" activeCellId="0" sqref="G113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1113,231 +1575,369 @@
       <c r="E1" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="H3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="3"/>
+      <c r="H4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="H5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="H6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="H8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="2"/>
+        <v>47</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="H9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="H10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="2"/>
+        <v>53</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="H11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="H12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="H13" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="2"/>
+        <v>68</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="2"/>
+        <v>67</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="H16" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="2"/>
+        <v>77</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="2" t="n">
+        <v>81</v>
+      </c>
+      <c r="E18" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1347,193 +1947,289 @@
         <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>55</v>
+        <v>93</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="H22" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>59</v>
+        <v>103</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>60</v>
+        <v>104</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="H23" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>61</v>
+        <v>107</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>62</v>
+        <v>108</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E24" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="H24" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>63</v>
+        <v>111</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E25" s="2"/>
+        <v>112</v>
+      </c>
+      <c r="E25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E26" s="2"/>
+        <v>114</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="H26" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>67</v>
+        <v>116</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>68</v>
+        <v>117</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E27" s="2"/>
+        <v>113</v>
+      </c>
+      <c r="E27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>69</v>
+        <v>118</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E28" s="2"/>
+        <v>119</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="H28" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>71</v>
+        <v>121</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E29" s="2"/>
+        <v>122</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="H29" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>74</v>
+        <v>125</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E30" s="2"/>
+        <v>121</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="H30" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>75</v>
+        <v>128</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>76</v>
+        <v>129</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E31" s="2"/>
+        <v>121</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>77</v>
+        <v>134</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>78</v>
+        <v>135</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1541,10 +2237,16 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>79</v>
+        <v>137</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>80</v>
+        <v>138</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1552,13 +2254,19 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>81</v>
+        <v>140</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>82</v>
+        <v>141</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>79</v>
+        <v>137</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1566,13 +2274,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>83</v>
+        <v>144</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>84</v>
+        <v>145</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>79</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1580,13 +2288,13 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>85</v>
+        <v>146</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>86</v>
+        <v>147</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>79</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1594,13 +2302,19 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>87</v>
+        <v>148</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>88</v>
+        <v>149</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>79</v>
+        <v>137</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1608,10 +2322,10 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>89</v>
+        <v>152</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>90</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1619,10 +2333,16 @@
         <v>4</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>91</v>
+        <v>154</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>92</v>
+        <v>155</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1630,10 +2350,10 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>94</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1641,10 +2361,16 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>95</v>
+        <v>160</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>96</v>
+        <v>161</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1652,10 +2378,16 @@
         <v>4</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>97</v>
+        <v>163</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>98</v>
+        <v>164</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1663,10 +2395,10 @@
         <v>4</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>99</v>
+        <v>167</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>100</v>
+        <v>168</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1674,10 +2406,10 @@
         <v>4</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>101</v>
+        <v>169</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>102</v>
+        <v>170</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1685,10 +2417,16 @@
         <v>4</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>103</v>
+        <v>171</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>104</v>
+        <v>172</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1696,10 +2434,10 @@
         <v>4</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>105</v>
+        <v>175</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>106</v>
+        <v>176</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1707,10 +2445,10 @@
         <v>4</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>107</v>
+        <v>177</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>108</v>
+        <v>178</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1718,13 +2456,13 @@
         <v>4</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>109</v>
+        <v>179</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>110</v>
+        <v>180</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>77</v>
+        <v>134</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1732,13 +2470,13 @@
         <v>4</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>111</v>
+        <v>181</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>112</v>
+        <v>182</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>79</v>
+        <v>137</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1746,10 +2484,10 @@
         <v>4</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>113</v>
+        <v>183</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>114</v>
+        <v>184</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1757,10 +2495,10 @@
         <v>4</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>115</v>
+        <v>185</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>116</v>
+        <v>186</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1768,10 +2506,10 @@
         <v>4</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>117</v>
+        <v>187</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>118</v>
+        <v>188</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1779,10 +2517,10 @@
         <v>4</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>120</v>
+        <v>189</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1790,10 +2528,16 @@
         <v>6</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>121</v>
+        <v>190</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>122</v>
+        <v>191</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="I54" s="6" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1801,10 +2545,16 @@
         <v>6</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>123</v>
+        <v>194</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>124</v>
+        <v>195</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="I55" s="6" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1812,10 +2562,16 @@
         <v>6</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>125</v>
+        <v>198</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>126</v>
+        <v>199</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="I56" s="6" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1823,10 +2579,16 @@
         <v>6</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>127</v>
+        <v>202</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>128</v>
+        <v>203</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="I57" s="6" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1834,10 +2596,10 @@
         <v>6</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>129</v>
+        <v>206</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>130</v>
+        <v>207</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1845,10 +2607,16 @@
         <v>6</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>131</v>
+        <v>208</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>132</v>
+        <v>209</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="I59" s="5" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1856,10 +2624,10 @@
         <v>6</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>133</v>
+        <v>212</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>134</v>
+        <v>213</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1867,10 +2635,22 @@
         <v>8</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>135</v>
+        <v>214</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>136</v>
+        <v>215</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="I61" s="6" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1878,10 +2658,22 @@
         <v>8</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>137</v>
+        <v>219</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>138</v>
+        <v>220</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="I62" s="6" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1889,10 +2681,16 @@
         <v>8</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>139</v>
+        <v>223</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>140</v>
+        <v>224</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1900,10 +2698,16 @@
         <v>8</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>141</v>
+        <v>226</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>142</v>
+        <v>227</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="I64" s="6" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1911,10 +2715,22 @@
         <v>8</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>143</v>
+        <v>229</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>144</v>
+        <v>230</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="I65" s="6" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1922,10 +2738,22 @@
         <v>8</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>145</v>
+        <v>233</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>146</v>
+        <v>234</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H66" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="I66" s="6" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1933,10 +2761,16 @@
         <v>8</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>147</v>
+        <v>237</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>148</v>
+        <v>238</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="I67" s="6" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1944,10 +2778,22 @@
         <v>8</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>149</v>
+        <v>240</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>150</v>
+        <v>241</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="I68" s="6" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1955,10 +2801,16 @@
         <v>8</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>151</v>
+        <v>244</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>152</v>
+        <v>245</v>
+      </c>
+      <c r="H69" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="I69" s="6" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1966,13 +2818,19 @@
         <v>8</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>153</v>
+        <v>247</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>154</v>
+        <v>248</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>135</v>
+        <v>214</v>
+      </c>
+      <c r="H70" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="I70" s="5" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1980,13 +2838,25 @@
         <v>8</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>155</v>
+        <v>250</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>156</v>
+        <v>251</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>135</v>
+        <v>214</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="G71" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="H71" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="I71" s="5" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1994,13 +2864,19 @@
         <v>8</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>157</v>
+        <v>254</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>158</v>
+        <v>255</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>135</v>
+        <v>214</v>
+      </c>
+      <c r="H72" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="I72" s="6" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2008,13 +2884,25 @@
         <v>8</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>159</v>
+        <v>257</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>160</v>
+        <v>258</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>135</v>
+        <v>214</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="G73" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="H73" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="I73" s="6" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2022,13 +2910,19 @@
         <v>8</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>161</v>
+        <v>261</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>162</v>
+        <v>262</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>137</v>
+        <v>219</v>
+      </c>
+      <c r="H74" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="I74" s="6" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2036,13 +2930,19 @@
         <v>8</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>163</v>
+        <v>265</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>164</v>
+        <v>266</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>137</v>
+        <v>219</v>
+      </c>
+      <c r="H75" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="I75" s="6" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2050,13 +2950,19 @@
         <v>8</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>165</v>
+        <v>269</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>166</v>
+        <v>270</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>137</v>
+        <v>219</v>
+      </c>
+      <c r="H76" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="I76" s="6" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2064,13 +2970,19 @@
         <v>8</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>167</v>
+        <v>273</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>168</v>
+        <v>274</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>139</v>
+        <v>223</v>
+      </c>
+      <c r="H77" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="I77" s="6" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2078,13 +2990,19 @@
         <v>8</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>169</v>
+        <v>276</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>170</v>
+        <v>277</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>139</v>
+        <v>223</v>
+      </c>
+      <c r="H78" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="I78" s="6" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2092,13 +3010,19 @@
         <v>8</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>171</v>
+        <v>279</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>172</v>
+        <v>280</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>141</v>
+        <v>226</v>
+      </c>
+      <c r="H79" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="I79" s="6" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2106,13 +3030,19 @@
         <v>8</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>173</v>
+        <v>283</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>174</v>
+        <v>284</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>141</v>
+        <v>226</v>
+      </c>
+      <c r="H80" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="I80" s="6" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2120,13 +3050,19 @@
         <v>8</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>175</v>
+        <v>287</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>176</v>
+        <v>288</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>141</v>
+        <v>226</v>
+      </c>
+      <c r="H81" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="I81" s="6" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2134,13 +3070,19 @@
         <v>8</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>177</v>
+        <v>291</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>178</v>
+        <v>292</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>143</v>
+        <v>229</v>
+      </c>
+      <c r="H82" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="I82" s="6" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2148,13 +3090,13 @@
         <v>8</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>179</v>
+        <v>295</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>180</v>
+        <v>296</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>143</v>
+        <v>229</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2162,13 +3104,13 @@
         <v>8</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>181</v>
+        <v>297</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>182</v>
+        <v>298</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>143</v>
+        <v>229</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2176,13 +3118,19 @@
         <v>8</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>183</v>
+        <v>299</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>184</v>
+        <v>300</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>143</v>
+        <v>229</v>
+      </c>
+      <c r="H85" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="I85" s="6" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2190,13 +3138,19 @@
         <v>8</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>185</v>
+        <v>303</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>186</v>
+        <v>304</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>145</v>
+        <v>233</v>
+      </c>
+      <c r="H86" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="I86" s="6" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2204,13 +3158,19 @@
         <v>8</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>187</v>
+        <v>307</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>188</v>
+        <v>308</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>145</v>
+        <v>233</v>
+      </c>
+      <c r="H87" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="I87" s="6" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2218,13 +3178,19 @@
         <v>8</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>189</v>
+        <v>311</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>190</v>
+        <v>312</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>145</v>
+        <v>233</v>
+      </c>
+      <c r="H88" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="I88" s="6" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2232,13 +3198,19 @@
         <v>8</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>191</v>
+        <v>315</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>192</v>
+        <v>316</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>145</v>
+        <v>233</v>
+      </c>
+      <c r="H89" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="I89" s="6" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2246,13 +3218,19 @@
         <v>8</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>193</v>
+        <v>319</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>194</v>
+        <v>320</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>147</v>
+        <v>237</v>
+      </c>
+      <c r="H90" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="I90" s="6" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2260,13 +3238,19 @@
         <v>8</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>195</v>
+        <v>322</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>196</v>
+        <v>323</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>147</v>
+        <v>237</v>
+      </c>
+      <c r="H91" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="I91" s="6" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2274,13 +3258,19 @@
         <v>8</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>197</v>
+        <v>325</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>198</v>
+        <v>326</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>149</v>
+        <v>240</v>
+      </c>
+      <c r="H92" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="I92" s="6" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2288,13 +3278,19 @@
         <v>8</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>199</v>
+        <v>329</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>200</v>
+        <v>330</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>149</v>
+        <v>240</v>
+      </c>
+      <c r="H93" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="I93" s="6" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2302,13 +3298,19 @@
         <v>8</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>201</v>
+        <v>333</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>202</v>
+        <v>334</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>149</v>
+        <v>240</v>
+      </c>
+      <c r="H94" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="I94" s="6" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2316,13 +3318,19 @@
         <v>8</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>203</v>
+        <v>337</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>204</v>
+        <v>338</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>149</v>
+        <v>240</v>
+      </c>
+      <c r="H95" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="I95" s="6" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2330,13 +3338,19 @@
         <v>8</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>205</v>
+        <v>340</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>206</v>
+        <v>341</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>149</v>
+        <v>240</v>
+      </c>
+      <c r="H96" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="I96" s="6" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2344,13 +3358,13 @@
         <v>8</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>207</v>
+        <v>344</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>208</v>
+        <v>345</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>149</v>
+        <v>240</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2358,13 +3372,13 @@
         <v>8</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>209</v>
+        <v>346</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>210</v>
+        <v>347</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>149</v>
+        <v>240</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2372,13 +3386,22 @@
         <v>8</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>211</v>
+        <v>348</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>212</v>
+        <v>349</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>151</v>
+        <v>244</v>
+      </c>
+      <c r="F99" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="H99" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="I99" s="6" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2386,13 +3409,25 @@
         <v>8</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>213</v>
+        <v>351</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>214</v>
+        <v>352</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>151</v>
+        <v>244</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="G100" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="H100" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="I100" s="6" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2400,13 +3435,25 @@
         <v>8</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>215</v>
+        <v>355</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>216</v>
+        <v>356</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>151</v>
+        <v>244</v>
+      </c>
+      <c r="F101" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="G101" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="H101" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="I101" s="6" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2414,13 +3461,25 @@
         <v>8</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>217</v>
+        <v>359</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>218</v>
+        <v>360</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>151</v>
+        <v>244</v>
+      </c>
+      <c r="F102" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="G102" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="H102" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="I102" s="6" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2428,13 +3487,13 @@
         <v>8</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>219</v>
+        <v>363</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>220</v>
+        <v>364</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>151</v>
+        <v>244</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2442,10 +3501,10 @@
         <v>10</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>221</v>
+        <v>365</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>222</v>
+        <v>366</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2453,10 +3512,10 @@
         <v>12</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>223</v>
+        <v>367</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>224</v>
+        <v>368</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2464,13 +3523,13 @@
         <v>12</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>225</v>
+        <v>369</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>225</v>
+        <v>369</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>223</v>
+        <v>367</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2478,13 +3537,13 @@
         <v>12</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>226</v>
+        <v>370</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>226</v>
+        <v>370</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>223</v>
+        <v>367</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2492,13 +3551,13 @@
         <v>12</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>227</v>
+        <v>371</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>228</v>
+        <v>372</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>223</v>
+        <v>367</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2506,13 +3565,13 @@
         <v>12</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>229</v>
+        <v>373</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>229</v>
+        <v>373</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>223</v>
+        <v>367</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2520,16 +3579,109 @@
         <v>12</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>230</v>
+        <v>374</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>231</v>
+        <v>375</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>223</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" display="https://lexicon.hum.uu.nl/zoek.pl?lemma=Noun+(N)&amp;lemmacode=509"/>
+    <hyperlink ref="I2" r:id="rId2" display="http://hdl.handle.net/11459/CCR_C-3347_7face0f5-7a72-7ec2-c988-7adba256cea9"/>
+    <hyperlink ref="I3" r:id="rId3" display="http://hdl.handle.net/11459/CCR_C-1371_fbebd9ec-a7f4-9a36-d6e9-88ee16b944ae "/>
+    <hyperlink ref="I4" r:id="rId4" display="http://hdl.handle.net/11459/CCR_C-385_d5af2f91-c926-3747-cc35-1d21aefd2717 "/>
+    <hyperlink ref="I5" r:id="rId5" display="http://hdl.handle.net/11459/CCR_C-1424_dc8402e6-a042-2d8a-4740-0d6cfe5ede02"/>
+    <hyperlink ref="I6" r:id="rId6" display="http://hdl.handle.net/11459/CCR_C-4948_ed655357-4652-f480-1a1e-a2999b785608"/>
+    <hyperlink ref="G7" r:id="rId7" display="https://lexicon.hum.uu.nl/zoek.pl?lemma=Adverb&amp;lemmacode=992"/>
+    <hyperlink ref="I7" r:id="rId8" display="http://hdl.handle.net/11459/CCR_C-4955_80fe4ee9-ea7e-527a-a860-b7956c95e1f8"/>
+    <hyperlink ref="I8" r:id="rId9" display="http://hdl.handle.net/11459/CCR_C-3419_28e9d227-d7f2-1ef7-a8a6-064c04dbdb4e"/>
+    <hyperlink ref="I9" r:id="rId10" display="http://hdl.handle.net/11459/CCR_C-1231_254a8099-18bf-fd87-781e-9dd5e5129c37"/>
+    <hyperlink ref="I10" r:id="rId11" display="http://hdl.handle.net/11459/CCR_C-1360_dc07e05a-b7bf-7e3e-360b-3d1e2a5c1c7f"/>
+    <hyperlink ref="I11" r:id="rId12" display="http://hdl.handle.net/11459/CCR_C-1334_3ef89474-3670-161f-6212-beb82406bb75"/>
+    <hyperlink ref="I12" r:id="rId13" display="http://hdl.handle.net/11459/CCR_C-3103_2703f461-5695-5fe4-46bd-bcb6d40d19c0"/>
+    <hyperlink ref="I13" r:id="rId14" display="http://hdl.handle.net/11459/CCR_C-3361_1af3740e-1092-c02a-2038-9428ddcddd7b"/>
+    <hyperlink ref="G14" r:id="rId15" display="https://lexicon.hum.uu.nl/zoek.pl?lemma=Particle&amp;lemmacode=382"/>
+    <hyperlink ref="I14" r:id="rId16" display="http://hdl.handle.net/11459/CCR_C-3372_8d6a8199-b259-537e-fbca-5de0aa46d7f9"/>
+    <hyperlink ref="G15" r:id="rId17" display="https://lexicon.hum.uu.nl/zoek.pl?lemma=Pronominal&amp;lemmacode=447"/>
+    <hyperlink ref="I15" r:id="rId18" display="http://hdl.handle.net/11459/CCR_C-4951_3b095c38-b7d9-6903-267b-5ab6a7812459"/>
+    <hyperlink ref="I16" r:id="rId19" display="http://hdl.handle.net/11459/CCR_C-1463_f07c7667-e90f-c10a-7239-1ecb8d804956 "/>
+    <hyperlink ref="G17" r:id="rId20" display="https://lexicon.hum.uu.nl/zoek.pl?lemma=Determiner&amp;lemmacode=1079"/>
+    <hyperlink ref="I17" r:id="rId21" display="http://hdl.handle.net/11459/CCR_C-3159_a027395b-0971-f4d3-52d5-f42dd670a655"/>
+    <hyperlink ref="G19" r:id="rId22" display="https://lexicon.hum.uu.nl/zoek.pl?lemma=Relative+pronoun&amp;lemmacode=332"/>
+    <hyperlink ref="I19" r:id="rId23" display="http://hdl.handle.net/11459/CCR_C-1380_e55f8cdf-1792-eb7a-6792-4e6c9b3c176a"/>
+    <hyperlink ref="G20" r:id="rId24" display="https://lexicon.hum.uu.nl/zoek.pl?lemma=Reflexive&amp;lemmacode=329"/>
+    <hyperlink ref="I20" r:id="rId25" display="http://hdl.handle.net/11459/CCR_C-3014_e837f69a-cc20-0fe6-a94a-153e8f59b694"/>
+    <hyperlink ref="G21" r:id="rId26" display="https://lexicon.hum.uu.nl/zoek.pl?lemma=Reciprocal&amp;lemmacode=316"/>
+    <hyperlink ref="I21" r:id="rId27" display="http://hdl.handle.net/11459/CCR_C-4986_c70204a7-79a7-b916-3cfb-1572cde565f8"/>
+    <hyperlink ref="I22" r:id="rId28" display="http://hdl.handle.net/11459/CCR_C-1270_bfb2e942-c2a8-1035-cde9-b8ada8c9aa70"/>
+    <hyperlink ref="I23" r:id="rId29" display="http://hdl.handle.net/11459/CCR_C-1321_35cb0c2b-aa78-024b-9e6b-ae2a94cb191c"/>
+    <hyperlink ref="I24" r:id="rId30" display="http://hdl.handle.net/11459/CCR_C-1359_41a180fd-f9a4-25e3-25c1-69c1225c31c8 "/>
+    <hyperlink ref="I26" r:id="rId31" display="http://hdl.handle.net/11459/CCR_C-5037_12ebd479-c44e-1e62-938e-38890ca17ef0"/>
+    <hyperlink ref="I28" r:id="rId32" display="http://hdl.handle.net/11459/CCR_C-3266_382e27ef-820b-8861-5aa3-b60dbe69936e"/>
+    <hyperlink ref="I29" r:id="rId33" display="http://hdl.handle.net/11459/CCR_C-3132_60542513-24d3-973f-9dd6-678d372e5aa7"/>
+    <hyperlink ref="I30" r:id="rId34" display="http://hdl.handle.net/11459/CCR_C-1262_64a7cd7c-4e1e-ac0a-0ee0-ac1541f27aea"/>
+    <hyperlink ref="G31" r:id="rId35" display="https://lexicon.hum.uu.nl/zoek.pl?lemma=Complementizer&amp;lemmacode=892"/>
+    <hyperlink ref="I31" r:id="rId36" display="http://hdl.handle.net/11459/CCR_C-1393_9905e94f-5624-ed01-139f-fc3ffac7a923"/>
+    <hyperlink ref="G32" r:id="rId37" display="https://lexicon.hum.uu.nl/zoek.pl?lemma=Subject&amp;lemmacode=285"/>
+    <hyperlink ref="G33" r:id="rId38" display="https://lexicon.hum.uu.nl/zoek.pl?lemma=Object&amp;lemmacode=462"/>
+    <hyperlink ref="I34" r:id="rId39" display="http://hdl.handle.net/11459/CCR_C-1274_2d458147-53dc-9010-d77b-3a3d6a0aeb49"/>
+    <hyperlink ref="I37" r:id="rId40" display="http://hdl.handle.net/11459/CCR_C-1310_ab441fcb-3588-e2c8-14ed-45e22106df1f"/>
+    <hyperlink ref="I39" r:id="rId41" display="http://hdl.handle.net/11459/CCR_C-4638_49e9d219-69c9-5391-2c85-67ae442761d6"/>
+    <hyperlink ref="I42" r:id="rId42" display="http://hdl.handle.net/11459/CCR_C-5454_aea7d73d-4cd2-4e36-0229-a009162e05ce"/>
+    <hyperlink ref="I54" r:id="rId43" display="http://hdl.handle.net/11459/CCR_C-2256_f31b9b2c-03a2-2251-10d4-7d98ddc042b0"/>
+    <hyperlink ref="I55" r:id="rId44" display="http://hdl.handle.net/11459/CCR_C-2258_121366f1-07d0-2c34-373d-342e4d637446 "/>
+    <hyperlink ref="I56" r:id="rId45" display="http://hdl.handle.net/11459/CCR_C-5768_1e635399-e84b-b206-6ece-4e573a30ca18 "/>
+    <hyperlink ref="I57" r:id="rId46" display="http://hdl.handle.net/11459/CCR_C-2255_88b411af-49bf-1cdb-7aad-224eb27ef06f"/>
+    <hyperlink ref="G61" r:id="rId47" display="https://lexicon.hum.uu.nl/zoek.pl?lemma=Mood&amp;lemmacode=559 "/>
+    <hyperlink ref="I61" r:id="rId48" display="http://hdl.handle.net/11459/CCR_C-1427_a6c3919f-4cc1-9d38-f431-3f44e45d0104 "/>
+    <hyperlink ref="G62" r:id="rId49" display="https://lexicon.hum.uu.nl/zoek.pl?lemma=Tense&amp;lemmacode=144"/>
+    <hyperlink ref="I62" r:id="rId50" display="http://hdl.handle.net/11459/CCR_C-1286_6bf93a88-ee71-1487-5de5-d7ca9c1f4397 "/>
+    <hyperlink ref="G63" r:id="rId51" display="https://lexicon.hum.uu.nl/zoek.pl?lemma=Aspect&amp;lemmacode=1041"/>
+    <hyperlink ref="I64" r:id="rId52" display="http://hdl.handle.net/11459/CCR_C-2775_0d862930-ad75-39db-21c5-7aeeef08b3c3 "/>
+    <hyperlink ref="G65" r:id="rId53" display="https://lexicon.hum.uu.nl/zoek.pl?lemma=Number&amp;lemmacode=518"/>
+    <hyperlink ref="I65" r:id="rId54" display="http://hdl.handle.net/11459/CCR_C-2709_cb240da0-9009-d7cf-4a7d-76c82bd9d571 "/>
+    <hyperlink ref="G66" r:id="rId55" display="https://lexicon.hum.uu.nl/zoek.pl?lemma=Gender&amp;lemmacode=716"/>
+    <hyperlink ref="I66" r:id="rId56" display="http://hdl.handle.net/11459/CCR_C-4926_08350667-c77d-15cb-2273-066dfba297c4 "/>
+    <hyperlink ref="I67" r:id="rId57" display="http://hdl.handle.net/11459/CCR_C-1926_54336616-beda-d9e9-c1e8-28f8233e8f7f "/>
+    <hyperlink ref="G68" r:id="rId58" display="https://lexicon.hum.uu.nl/zoek.pl?lemma=Case&amp;lemmacode=854"/>
+    <hyperlink ref="I68" r:id="rId59" display="http://hdl.handle.net/11459/CCR_C-1840_9f4e319c-f233-6c90-9117-7270e215f039 "/>
+    <hyperlink ref="I69" r:id="rId60" display="http://hdl.handle.net/11459/CCR_C-4920_305a6674-d773-1ab4-2deb-66871c089fff "/>
+    <hyperlink ref="G71" r:id="rId61" display="https://lexicon.hum.uu.nl/zoek.pl?lemma=Subjunctive&amp;lemmacode=291"/>
+    <hyperlink ref="I72" r:id="rId62" display="http://hdl.handle.net/11459/CCR_C-4967_f065b067-9908-dfd2-9397-27261b8e17d0 "/>
+    <hyperlink ref="G73" r:id="rId63" display="https://lexicon.hum.uu.nl/zoek.pl?lemma=Imperative&amp;lemmacode=652"/>
+    <hyperlink ref="I73" r:id="rId64" display="http://hdl.handle.net/11459/CCR_C-1844_21036bac-13d1-18fc-ca4f-2590f5c84013 "/>
+    <hyperlink ref="I74" r:id="rId65" display="http://hdl.handle.net/11459/CCR_C-4965_703be00b-9336-3673-0f2d-d274352dd15e "/>
+    <hyperlink ref="I75" r:id="rId66" display="http://hdl.handle.net/11459/CCR_C-4966_7a720367-df40-f728-e11d-7504a03ec27b "/>
+    <hyperlink ref="I76" r:id="rId67" display="http://hdl.handle.net/11459/CCR_C-1291_c2896356-8d7e-e425-d2ac-5741e93db4e2 "/>
+    <hyperlink ref="I77" r:id="rId68" display="http://hdl.handle.net/11459/CCR_C-1305_7066f625-844d-7091-167c-1770bb560b7e "/>
+    <hyperlink ref="I78" r:id="rId69" display="http://hdl.handle.net/11459/CCR_C-1352_2664f3ef-8d98-764f-9ec5-d582ed04d312 "/>
+    <hyperlink ref="I79" r:id="rId70" display="http://hdl.handle.net/11459/CCR_C-1288_61cc5804-ed04-b31a-d550-7fe84a188345 "/>
+    <hyperlink ref="I80" r:id="rId71" display="http://hdl.handle.net/11459/CCR_C-1384_a6aa56c1-3f5d-901f-cbbb-ecc8fdce9d69 "/>
+    <hyperlink ref="I81" r:id="rId72" display="http://hdl.handle.net/11459/CCR_C-1402_fd8749a9-cd4a-530e-760e-17944acfd054 "/>
+    <hyperlink ref="I82" r:id="rId73" display="http://hdl.handle.net/11459/CCR_C-2707_9c804dcc-7939-8f37-d4d4-10423ee65e20 "/>
+    <hyperlink ref="I85" r:id="rId74" display="http://hdl.handle.net/11459/CCR_C-2708_74a6e5d5-6df6-7756-c882-ce09731285eb "/>
+    <hyperlink ref="I86" r:id="rId75" display="http://hdl.handle.net/11459/CCR_C-3312_4e7c6a3d-3b48-8ade-de52-cfaa9122269a "/>
+    <hyperlink ref="I87" r:id="rId76" display="http://hdl.handle.net/11459/CCR_C-3197_9e0c49be-b888-bc56-b6d1-05f4dd1d5a66 "/>
+    <hyperlink ref="I88" r:id="rId77" display="http://hdl.handle.net/11459/CCR_C-3336_086f7d13-1e1c-8618-5051-b9c7ab4cf860 "/>
+    <hyperlink ref="I89" r:id="rId78" display="http://hdl.handle.net/11459/CCR_C-1558_015e4ddd-aff5-d9ec-ec64-e6be2c029456 "/>
+    <hyperlink ref="I90" r:id="rId79" display="http://hdl.handle.net/11459/CCR_C-2004_7dc427d7-61a6-853e-12ea-c7f766afc5b6 "/>
+    <hyperlink ref="I91" r:id="rId80" display="http://hdl.handle.net/11459/CCR_C-2005_05c694a1-bf78-c5bc-4913-a87f7b30f251 "/>
+    <hyperlink ref="I92" r:id="rId81" display="http://hdl.handle.net/11459/CCR_C-1331_89e7297d-85b0-5391-ea92-92347358719d "/>
+    <hyperlink ref="I93" r:id="rId82" display="http://hdl.handle.net/11459/CCR_C-2724_53acfdbe-6741-7430-6e7f-677b47993c17 "/>
+    <hyperlink ref="I94" r:id="rId83" display="http://hdl.handle.net/11459/CCR_C-1293_5ce1a413-afaf-1ae5-f818-a416f219fc41 "/>
+    <hyperlink ref="I95" r:id="rId84" display="http://hdl.handle.net/11459/CCR_C-4938_8d013ba9-c95a-ec59-6cc9-ed61e2cff5f1 "/>
+    <hyperlink ref="I96" r:id="rId85" display="http://hdl.handle.net/11459/CCR_C-2726_da687347-23ae-062f-92c5-af3acf7d6b82 "/>
+    <hyperlink ref="I99" r:id="rId86" display="http://hdl.handle.net/11459/CCR_C-1420_745016c4-84c2-766a-a861-b4cdb6dcba73 "/>
+    <hyperlink ref="I100" r:id="rId87" display="http://hdl.handle.net/11459/CCR_C-4924_1867b087-ed2e-1641-4948-6753bc5c439a "/>
+    <hyperlink ref="G101" r:id="rId88" display="https://lexicon.hum.uu.nl/zoek.pl?lemma=Superlative&amp;lemmacode=299"/>
+    <hyperlink ref="I101" r:id="rId89" display="http://hdl.handle.net/11459/CCR_C-4925_fe8c3b92-8af1-70e2-2534-923b977ac4e8 "/>
+    <hyperlink ref="G102" r:id="rId90" display="https://lexicon.hum.uu.nl/zoek.pl?lemma=Diminutive&amp;lemmacode=1081"/>
+    <hyperlink ref="I102" r:id="rId91" display="http://hdl.handle.net/11459/CCR_C-3046_73e3fbc4-0fc7-513e-d225-517203331e74 "/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Add missing ULL URI for positive
</commit_message>
<xml_diff>
--- a/vocabulary/lexicon.xlsx
+++ b/vocabulary/lexicon.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="377">
   <si>
     <t xml:space="preserve">slug</t>
   </si>
@@ -1071,6 +1071,9 @@
   </si>
   <si>
     <t xml:space="preserve">Positive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://lexicon.hum.uu.nl/zoek.pl?lemma=positive</t>
   </si>
   <si>
     <t xml:space="preserve">http://hdl.handle.net/11459/CCR_C-1420_745016c4-84c2-766a-a861-b4cdb6dcba73 </t>
@@ -1238,7 +1241,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1256,10 +1259,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1545,9 +1544,9 @@
   <dimension ref="A1:I110"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G113" activeCellId="0" sqref="G113"/>
+      <selection pane="bottomLeft" activeCell="G99" activeCellId="0" sqref="G99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1588,7 +1587,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1605,14 +1604,14 @@
       <c r="G2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1626,14 +1625,14 @@
         <v>21</v>
       </c>
       <c r="E3" s="3"/>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1647,14 +1646,14 @@
         <v>21</v>
       </c>
       <c r="E4" s="3"/>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1665,14 +1664,14 @@
         <v>34</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1683,14 +1682,14 @@
         <v>37</v>
       </c>
       <c r="E6" s="3"/>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1707,14 +1706,14 @@
       <c r="G7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -1728,14 +1727,14 @@
         <v>45</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -1746,14 +1745,14 @@
         <v>47</v>
       </c>
       <c r="E9" s="3"/>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -1767,14 +1766,14 @@
         <v>45</v>
       </c>
       <c r="E10" s="3"/>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -1785,14 +1784,14 @@
         <v>53</v>
       </c>
       <c r="E11" s="3"/>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1806,14 +1805,14 @@
         <v>52</v>
       </c>
       <c r="E12" s="3"/>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -1827,14 +1826,14 @@
         <v>52</v>
       </c>
       <c r="E13" s="3"/>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -1851,14 +1850,14 @@
       <c r="G14" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="I14" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -1875,14 +1874,14 @@
       <c r="G15" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
@@ -1896,14 +1895,14 @@
         <v>67</v>
       </c>
       <c r="E16" s="3"/>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -1920,10 +1919,10 @@
       <c r="G17" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="4" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1942,7 +1941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -1956,20 +1955,20 @@
         <v>80</v>
       </c>
       <c r="E19" s="3"/>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="H19" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I19" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
@@ -1983,20 +1982,20 @@
         <v>80</v>
       </c>
       <c r="E20" s="3"/>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H20" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -2010,20 +2009,20 @@
         <v>80</v>
       </c>
       <c r="E21" s="3"/>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="H21" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="I21" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
@@ -2037,14 +2036,14 @@
         <v>80</v>
       </c>
       <c r="E22" s="3"/>
-      <c r="H22" s="5" t="s">
+      <c r="H22" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="I22" s="6" t="s">
+      <c r="I22" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
@@ -2058,14 +2057,14 @@
         <v>80</v>
       </c>
       <c r="E23" s="3"/>
-      <c r="H23" s="5" t="s">
+      <c r="H23" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="I23" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
@@ -2079,10 +2078,10 @@
         <v>80</v>
       </c>
       <c r="E24" s="3"/>
-      <c r="H24" s="5" t="s">
+      <c r="H24" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="I24" s="6" t="s">
+      <c r="I24" s="4" t="s">
         <v>110</v>
       </c>
     </row>
@@ -2098,7 +2097,7 @@
       </c>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
@@ -2109,10 +2108,10 @@
         <v>114</v>
       </c>
       <c r="E26" s="3"/>
-      <c r="H26" s="5" t="s">
+      <c r="H26" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I26" s="6" t="s">
+      <c r="I26" s="4" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2131,7 +2130,7 @@
       </c>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
@@ -2142,14 +2141,14 @@
         <v>119</v>
       </c>
       <c r="E28" s="3"/>
-      <c r="H28" s="5" t="s">
+      <c r="H28" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I28" s="6" t="s">
+      <c r="I28" s="4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>2</v>
       </c>
@@ -2160,14 +2159,14 @@
         <v>122</v>
       </c>
       <c r="E29" s="3"/>
-      <c r="H29" s="5" t="s">
+      <c r="H29" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="I29" s="6" t="s">
+      <c r="I29" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>2</v>
       </c>
@@ -2181,14 +2180,14 @@
         <v>121</v>
       </c>
       <c r="E30" s="3"/>
-      <c r="H30" s="5" t="s">
+      <c r="H30" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="I30" s="6" t="s">
+      <c r="I30" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
@@ -2208,14 +2207,14 @@
       <c r="G31" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="H31" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="I31" s="6" t="s">
+      <c r="I31" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>4</v>
       </c>
@@ -2232,7 +2231,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -2249,7 +2248,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>4</v>
       </c>
@@ -2262,10 +2261,10 @@
       <c r="D34" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="H34" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="I34" s="6" t="s">
+      <c r="I34" s="4" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2297,7 +2296,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>4</v>
       </c>
@@ -2310,10 +2309,10 @@
       <c r="D37" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="H37" s="5" t="s">
+      <c r="H37" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="I37" s="6" t="s">
+      <c r="I37" s="4" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2328,7 +2327,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>4</v>
       </c>
@@ -2338,10 +2337,10 @@
       <c r="C39" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="H39" s="5" t="s">
+      <c r="H39" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="I39" s="6" t="s">
+      <c r="I39" s="4" t="s">
         <v>157</v>
       </c>
     </row>
@@ -2373,7 +2372,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>4</v>
       </c>
@@ -2383,10 +2382,10 @@
       <c r="C42" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="H42" s="5" t="s">
+      <c r="H42" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="I42" s="6" t="s">
+      <c r="I42" s="4" t="s">
         <v>166</v>
       </c>
     </row>
@@ -2422,10 +2421,10 @@
       <c r="C45" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="H45" s="5" t="s">
+      <c r="H45" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="I45" s="5" t="s">
+      <c r="I45" s="2" t="s">
         <v>174</v>
       </c>
     </row>
@@ -2523,7 +2522,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
         <v>6</v>
       </c>
@@ -2533,14 +2532,14 @@
       <c r="C54" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="H54" s="5" t="s">
+      <c r="H54" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="I54" s="6" t="s">
+      <c r="I54" s="4" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
         <v>6</v>
       </c>
@@ -2550,14 +2549,14 @@
       <c r="C55" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="H55" s="5" t="s">
+      <c r="H55" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="I55" s="6" t="s">
+      <c r="I55" s="4" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>6</v>
       </c>
@@ -2567,14 +2566,14 @@
       <c r="C56" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="H56" s="5" t="s">
+      <c r="H56" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="I56" s="6" t="s">
+      <c r="I56" s="4" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
         <v>6</v>
       </c>
@@ -2584,10 +2583,10 @@
       <c r="C57" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="H57" s="5" t="s">
+      <c r="H57" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="I57" s="6" t="s">
+      <c r="I57" s="4" t="s">
         <v>205</v>
       </c>
     </row>
@@ -2612,10 +2611,10 @@
       <c r="C59" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="H59" s="5" t="s">
+      <c r="H59" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="I59" s="5" t="s">
+      <c r="I59" s="2" t="s">
         <v>211</v>
       </c>
     </row>
@@ -2630,7 +2629,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
         <v>8</v>
       </c>
@@ -2640,20 +2639,20 @@
       <c r="C61" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="F61" s="5" t="s">
+      <c r="F61" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="G61" s="6" t="s">
+      <c r="G61" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="H61" s="5" t="s">
+      <c r="H61" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="I61" s="6" t="s">
+      <c r="I61" s="4" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
         <v>8</v>
       </c>
@@ -2663,20 +2662,20 @@
       <c r="C62" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="F62" s="5" t="s">
+      <c r="F62" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="G62" s="6" t="s">
+      <c r="G62" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="H62" s="5" t="s">
+      <c r="H62" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="I62" s="6" t="s">
+      <c r="I62" s="4" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
         <v>8</v>
       </c>
@@ -2686,14 +2685,14 @@
       <c r="C63" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="F63" s="5" t="s">
+      <c r="F63" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="G63" s="6" t="s">
+      <c r="G63" s="4" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>8</v>
       </c>
@@ -2703,14 +2702,14 @@
       <c r="C64" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="H64" s="5" t="s">
+      <c r="H64" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="I64" s="6" t="s">
+      <c r="I64" s="4" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
         <v>8</v>
       </c>
@@ -2720,20 +2719,20 @@
       <c r="C65" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="F65" s="5" t="s">
+      <c r="F65" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="G65" s="6" t="s">
+      <c r="G65" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="H65" s="5" t="s">
+      <c r="H65" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="I65" s="6" t="s">
+      <c r="I65" s="4" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
         <v>8</v>
       </c>
@@ -2743,20 +2742,20 @@
       <c r="C66" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="F66" s="5" t="s">
+      <c r="F66" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="G66" s="6" t="s">
+      <c r="G66" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="H66" s="5" t="s">
+      <c r="H66" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="I66" s="6" t="s">
+      <c r="I66" s="4" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
         <v>8</v>
       </c>
@@ -2766,14 +2765,14 @@
       <c r="C67" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="H67" s="5" t="s">
+      <c r="H67" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="I67" s="6" t="s">
+      <c r="I67" s="4" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
         <v>8</v>
       </c>
@@ -2783,20 +2782,20 @@
       <c r="C68" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="F68" s="5" t="s">
+      <c r="F68" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="G68" s="6" t="s">
+      <c r="G68" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="H68" s="5" t="s">
+      <c r="H68" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="I68" s="6" t="s">
+      <c r="I68" s="4" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
         <v>8</v>
       </c>
@@ -2806,10 +2805,10 @@
       <c r="C69" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="H69" s="5" t="s">
+      <c r="H69" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="I69" s="6" t="s">
+      <c r="I69" s="4" t="s">
         <v>246</v>
       </c>
     </row>
@@ -2826,14 +2825,14 @@
       <c r="D70" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="H70" s="5" t="s">
+      <c r="H70" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="I70" s="5" t="s">
+      <c r="I70" s="2" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
         <v>8</v>
       </c>
@@ -2846,20 +2845,20 @@
       <c r="D71" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="F71" s="5" t="s">
+      <c r="F71" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="G71" s="6" t="s">
+      <c r="G71" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="H71" s="5" t="s">
+      <c r="H71" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="I71" s="5" t="s">
+      <c r="I71" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
         <v>8</v>
       </c>
@@ -2872,14 +2871,14 @@
       <c r="D72" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="H72" s="5" t="s">
+      <c r="H72" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="I72" s="6" t="s">
+      <c r="I72" s="4" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
         <v>8</v>
       </c>
@@ -2892,20 +2891,20 @@
       <c r="D73" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="F73" s="5" t="s">
+      <c r="F73" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="G73" s="6" t="s">
+      <c r="G73" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="H73" s="5" t="s">
+      <c r="H73" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="I73" s="6" t="s">
+      <c r="I73" s="4" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
         <v>8</v>
       </c>
@@ -2918,14 +2917,14 @@
       <c r="D74" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="H74" s="5" t="s">
+      <c r="H74" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="I74" s="6" t="s">
+      <c r="I74" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
         <v>8</v>
       </c>
@@ -2938,14 +2937,14 @@
       <c r="D75" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="H75" s="5" t="s">
+      <c r="H75" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="I75" s="6" t="s">
+      <c r="I75" s="4" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
         <v>8</v>
       </c>
@@ -2958,14 +2957,14 @@
       <c r="D76" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="H76" s="5" t="s">
+      <c r="H76" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="I76" s="6" t="s">
+      <c r="I76" s="4" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
         <v>8</v>
       </c>
@@ -2978,14 +2977,14 @@
       <c r="D77" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="H77" s="5" t="s">
+      <c r="H77" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="I77" s="6" t="s">
+      <c r="I77" s="4" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
         <v>8</v>
       </c>
@@ -2998,14 +2997,14 @@
       <c r="D78" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="H78" s="5" t="s">
+      <c r="H78" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="I78" s="6" t="s">
+      <c r="I78" s="4" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
         <v>8</v>
       </c>
@@ -3018,14 +3017,14 @@
       <c r="D79" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="H79" s="5" t="s">
+      <c r="H79" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="I79" s="6" t="s">
+      <c r="I79" s="4" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
         <v>8</v>
       </c>
@@ -3038,14 +3037,14 @@
       <c r="D80" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="H80" s="5" t="s">
+      <c r="H80" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="I80" s="6" t="s">
+      <c r="I80" s="4" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
         <v>8</v>
       </c>
@@ -3058,14 +3057,14 @@
       <c r="D81" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="H81" s="5" t="s">
+      <c r="H81" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="I81" s="6" t="s">
+      <c r="I81" s="4" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
         <v>8</v>
       </c>
@@ -3078,10 +3077,10 @@
       <c r="D82" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="H82" s="5" t="s">
+      <c r="H82" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="I82" s="6" t="s">
+      <c r="I82" s="4" t="s">
         <v>294</v>
       </c>
     </row>
@@ -3113,7 +3112,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
         <v>8</v>
       </c>
@@ -3126,14 +3125,14 @@
       <c r="D85" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="H85" s="5" t="s">
+      <c r="H85" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="I85" s="6" t="s">
+      <c r="I85" s="4" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
         <v>8</v>
       </c>
@@ -3146,14 +3145,14 @@
       <c r="D86" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H86" s="5" t="s">
+      <c r="H86" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="I86" s="6" t="s">
+      <c r="I86" s="4" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
         <v>8</v>
       </c>
@@ -3166,14 +3165,14 @@
       <c r="D87" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H87" s="5" t="s">
+      <c r="H87" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="I87" s="6" t="s">
+      <c r="I87" s="4" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
         <v>8</v>
       </c>
@@ -3186,14 +3185,14 @@
       <c r="D88" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H88" s="5" t="s">
+      <c r="H88" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="I88" s="6" t="s">
+      <c r="I88" s="4" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
         <v>8</v>
       </c>
@@ -3206,14 +3205,14 @@
       <c r="D89" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H89" s="5" t="s">
+      <c r="H89" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="I89" s="6" t="s">
+      <c r="I89" s="4" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
         <v>8</v>
       </c>
@@ -3226,14 +3225,14 @@
       <c r="D90" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="H90" s="5" t="s">
+      <c r="H90" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="I90" s="6" t="s">
+      <c r="I90" s="4" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
         <v>8</v>
       </c>
@@ -3246,14 +3245,14 @@
       <c r="D91" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="H91" s="5" t="s">
+      <c r="H91" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="I91" s="6" t="s">
+      <c r="I91" s="4" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
         <v>8</v>
       </c>
@@ -3266,14 +3265,14 @@
       <c r="D92" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="H92" s="5" t="s">
+      <c r="H92" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="I92" s="6" t="s">
+      <c r="I92" s="4" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
         <v>8</v>
       </c>
@@ -3286,14 +3285,14 @@
       <c r="D93" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="H93" s="5" t="s">
+      <c r="H93" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="I93" s="6" t="s">
+      <c r="I93" s="4" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
         <v>8</v>
       </c>
@@ -3306,14 +3305,14 @@
       <c r="D94" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="H94" s="5" t="s">
+      <c r="H94" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="I94" s="6" t="s">
+      <c r="I94" s="4" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
         <v>8</v>
       </c>
@@ -3326,14 +3325,14 @@
       <c r="D95" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="H95" s="5" t="s">
+      <c r="H95" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="I95" s="6" t="s">
+      <c r="I95" s="4" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
         <v>8</v>
       </c>
@@ -3346,10 +3345,10 @@
       <c r="D96" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="H96" s="5" t="s">
+      <c r="H96" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="I96" s="6" t="s">
+      <c r="I96" s="4" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3394,92 +3393,95 @@
       <c r="D99" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="F99" s="5" t="s">
+      <c r="F99" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="H99" s="5" t="s">
+      <c r="G99" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="H99" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="I99" s="6" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I99" s="4" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="F100" s="5" t="s">
-        <v>351</v>
-      </c>
-      <c r="G100" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="H100" s="5" t="s">
-        <v>351</v>
-      </c>
-      <c r="I100" s="6" t="s">
+      <c r="F100" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="G100" s="2" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H100" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="I100" s="4" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="F101" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="G101" s="6" t="s">
-        <v>357</v>
-      </c>
-      <c r="H101" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="I101" s="6" t="s">
+      <c r="F101" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="G101" s="4" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H101" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="I101" s="4" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="F102" s="5" t="s">
-        <v>359</v>
-      </c>
-      <c r="G102" s="6" t="s">
-        <v>361</v>
-      </c>
-      <c r="H102" s="5" t="s">
-        <v>359</v>
-      </c>
-      <c r="I102" s="6" t="s">
+      <c r="F102" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="G102" s="4" t="s">
         <v>362</v>
+      </c>
+      <c r="H102" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="I102" s="4" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3487,10 +3489,10 @@
         <v>8</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>244</v>
@@ -3501,10 +3503,10 @@
         <v>10</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3512,10 +3514,10 @@
         <v>12</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3523,13 +3525,13 @@
         <v>12</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3537,13 +3539,13 @@
         <v>12</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3551,13 +3553,13 @@
         <v>12</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3565,13 +3567,13 @@
         <v>12</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3579,13 +3581,13 @@
         <v>12</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>
@@ -3675,12 +3677,13 @@
     <hyperlink ref="I94" r:id="rId83" display="http://hdl.handle.net/11459/CCR_C-1293_5ce1a413-afaf-1ae5-f818-a416f219fc41 "/>
     <hyperlink ref="I95" r:id="rId84" display="http://hdl.handle.net/11459/CCR_C-4938_8d013ba9-c95a-ec59-6cc9-ed61e2cff5f1 "/>
     <hyperlink ref="I96" r:id="rId85" display="http://hdl.handle.net/11459/CCR_C-2726_da687347-23ae-062f-92c5-af3acf7d6b82 "/>
-    <hyperlink ref="I99" r:id="rId86" display="http://hdl.handle.net/11459/CCR_C-1420_745016c4-84c2-766a-a861-b4cdb6dcba73 "/>
-    <hyperlink ref="I100" r:id="rId87" display="http://hdl.handle.net/11459/CCR_C-4924_1867b087-ed2e-1641-4948-6753bc5c439a "/>
-    <hyperlink ref="G101" r:id="rId88" display="https://lexicon.hum.uu.nl/zoek.pl?lemma=Superlative&amp;lemmacode=299"/>
-    <hyperlink ref="I101" r:id="rId89" display="http://hdl.handle.net/11459/CCR_C-4925_fe8c3b92-8af1-70e2-2534-923b977ac4e8 "/>
-    <hyperlink ref="G102" r:id="rId90" display="https://lexicon.hum.uu.nl/zoek.pl?lemma=Diminutive&amp;lemmacode=1081"/>
-    <hyperlink ref="I102" r:id="rId91" display="http://hdl.handle.net/11459/CCR_C-3046_73e3fbc4-0fc7-513e-d225-517203331e74 "/>
+    <hyperlink ref="G99" r:id="rId86" display="https://lexicon.hum.uu.nl/zoek.pl?lemma=positive"/>
+    <hyperlink ref="I99" r:id="rId87" display="http://hdl.handle.net/11459/CCR_C-1420_745016c4-84c2-766a-a861-b4cdb6dcba73 "/>
+    <hyperlink ref="I100" r:id="rId88" display="http://hdl.handle.net/11459/CCR_C-4924_1867b087-ed2e-1641-4948-6753bc5c439a "/>
+    <hyperlink ref="G101" r:id="rId89" display="https://lexicon.hum.uu.nl/zoek.pl?lemma=Superlative&amp;lemmacode=299"/>
+    <hyperlink ref="I101" r:id="rId90" display="http://hdl.handle.net/11459/CCR_C-4925_fe8c3b92-8af1-70e2-2534-923b977ac4e8 "/>
+    <hyperlink ref="G102" r:id="rId91" display="https://lexicon.hum.uu.nl/zoek.pl?lemma=Diminutive&amp;lemmacode=1081"/>
+    <hyperlink ref="I102" r:id="rId92" display="http://hdl.handle.net/11459/CCR_C-3046_73e3fbc4-0fc7-513e-d225-517203331e74 "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>